<commit_message>
Revert "my third commit"
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -113,7 +113,7 @@
     <t>1. Приложение установлено на ПК</t>
   </si>
   <si>
-    <t>2. увдлоудлоумдулвльджусуджсбус</t>
+    <t xml:space="preserve">2. </t>
   </si>
   <si>
     <t xml:space="preserve">3. </t>
@@ -3327,8 +3327,8 @@
   <sheetPr/>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A8" sqref="A7:J251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Revert "Revert "my third commit""
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -113,7 +113,7 @@
     <t>1. Приложение установлено на ПК</t>
   </si>
   <si>
-    <t xml:space="preserve">2. </t>
+    <t>2. увдлоудлоумдулвльджусуджсбус</t>
   </si>
   <si>
     <t xml:space="preserve">3. </t>
@@ -3327,8 +3327,8 @@
   <sheetPr/>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A7:J251"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>